<commit_message>
enhance CFG generation for more cases
</commit_message>
<xml_diff>
--- a/LoggingSyntaxAnalysis.xlsx
+++ b/LoggingSyntaxAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shuo_\eclipse-workspace2\COMP490\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191E4ADB-3D6A-4BAB-8945-E2104F047D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312F3704-0394-4632-8FEA-ECE10F867018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15930" xr2:uid="{B85E14B9-CD1F-4FBE-B3AD-3B561A4F1D46}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{B85E14B9-CD1F-4FBE-B3AD-3B561A4F1D46}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -621,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB8EBEA-9FCA-4311-BD9F-D1F800540DF8}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>